<commit_message>
Reading in mass parameters from master titration file
</commit_message>
<xml_diff>
--- a/Master_Tit_File.xlsx
+++ b/Master_Tit_File.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ct6g18/Python/org-alk-sausage-machine/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56DD4C29-7537-CA43-B528-34B621644EE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66FFC717-CDC4-2649-876B-5BA772EBED4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="20">
   <si>
     <t>tests/data/</t>
   </si>
@@ -40,9 +40,6 @@
     <t>seawater-CRM-144.dat</t>
   </si>
   <si>
-    <t>NaN</t>
-  </si>
-  <si>
     <t>g_0</t>
   </si>
   <si>
@@ -83,15 +80,6 @@
   </si>
   <si>
     <t>This is the file name (should be a .xlsx)</t>
-  </si>
-  <si>
-    <t>01.09.21.50UM.001_PROCESSED.xlsx,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">                            "01.09.21.50UM.001.NAOH_PROCESSED.xlsx",</t>
-  </si>
-  <si>
-    <t xml:space="preserve">                            "01.09.21.50UM.001.BT_PROCESSED.xlsx"</t>
   </si>
   <si>
     <t>01.09.21.50UM.001.BT_PROCESSED.xlsx</t>
@@ -944,10 +932,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L22"/>
+  <dimension ref="A1:L10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+      <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -964,48 +952,48 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" t="s">
         <v>7</v>
       </c>
-      <c r="B1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>9</v>
       </c>
-      <c r="G1" t="s">
-        <v>8</v>
-      </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>10</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>11</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>12</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>13</v>
-      </c>
-      <c r="L1" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B2" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C2">
         <v>33.570999999999998</v>
@@ -1013,8 +1001,8 @@
       <c r="E2">
         <v>100</v>
       </c>
-      <c r="F2" t="s">
-        <v>2</v>
+      <c r="F2">
+        <v>10</v>
       </c>
       <c r="G2">
         <v>2031.53</v>
@@ -1025,16 +1013,22 @@
       <c r="I2">
         <v>2.5</v>
       </c>
+      <c r="J2">
+        <v>0.21</v>
+      </c>
+      <c r="K2">
+        <v>3.5</v>
+      </c>
       <c r="L2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B3" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C3">
         <v>33.573</v>
@@ -1042,8 +1036,8 @@
       <c r="E3">
         <v>1000</v>
       </c>
-      <c r="F3" t="s">
-        <v>2</v>
+      <c r="F3">
+        <v>10</v>
       </c>
       <c r="G3">
         <v>2031.53</v>
@@ -1054,16 +1048,22 @@
       <c r="I3">
         <v>2.5</v>
       </c>
+      <c r="J3">
+        <v>0.21</v>
+      </c>
+      <c r="K3">
+        <v>3.5</v>
+      </c>
       <c r="L3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B4" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C4">
         <v>33.570999999999998</v>
@@ -1071,8 +1071,8 @@
       <c r="E4">
         <v>100</v>
       </c>
-      <c r="F4" t="s">
-        <v>2</v>
+      <c r="F4">
+        <v>10</v>
       </c>
       <c r="G4">
         <v>2031.53</v>
@@ -1083,8 +1083,14 @@
       <c r="I4">
         <v>2.5</v>
       </c>
+      <c r="J4">
+        <v>0.21</v>
+      </c>
+      <c r="K4">
+        <v>3.5</v>
+      </c>
       <c r="L4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
@@ -1100,8 +1106,8 @@
       <c r="E5">
         <v>100</v>
       </c>
-      <c r="F5" t="s">
-        <v>2</v>
+      <c r="F5">
+        <v>10</v>
       </c>
       <c r="G5">
         <v>2031.53</v>
@@ -1112,8 +1118,14 @@
       <c r="I5">
         <v>2.5</v>
       </c>
+      <c r="J5">
+        <v>0.21</v>
+      </c>
+      <c r="K5">
+        <v>3.5</v>
+      </c>
       <c r="L5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
@@ -1129,8 +1141,8 @@
       <c r="E6">
         <v>100</v>
       </c>
-      <c r="F6" t="s">
-        <v>2</v>
+      <c r="F6">
+        <v>10</v>
       </c>
       <c r="G6">
         <v>2031.53</v>
@@ -1141,8 +1153,14 @@
       <c r="I6">
         <v>2.5</v>
       </c>
+      <c r="J6">
+        <v>0.21</v>
+      </c>
+      <c r="K6">
+        <v>3.5</v>
+      </c>
       <c r="L6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
@@ -1158,8 +1176,8 @@
       <c r="E7">
         <v>100</v>
       </c>
-      <c r="F7" t="s">
-        <v>2</v>
+      <c r="F7">
+        <v>10</v>
       </c>
       <c r="G7">
         <v>2031.53</v>
@@ -1170,8 +1188,14 @@
       <c r="I7">
         <v>2.5</v>
       </c>
+      <c r="J7">
+        <v>0.21</v>
+      </c>
+      <c r="K7">
+        <v>3.5</v>
+      </c>
       <c r="L7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
@@ -1187,8 +1211,8 @@
       <c r="E8">
         <v>100</v>
       </c>
-      <c r="F8" t="s">
-        <v>2</v>
+      <c r="F8">
+        <v>10</v>
       </c>
       <c r="G8">
         <v>2031.53</v>
@@ -1199,28 +1223,19 @@
       <c r="I8">
         <v>2.5</v>
       </c>
+      <c r="J8">
+        <v>0.21</v>
+      </c>
+      <c r="K8">
+        <v>3.5</v>
+      </c>
       <c r="L8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B20" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B21" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B22" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated master titration file
</commit_message>
<xml_diff>
--- a/Master_Tit_File.xlsx
+++ b/Master_Tit_File.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ct6g18/Python/org-alk-sausage-machine/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66FFC717-CDC4-2649-876B-5BA772EBED4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92EA2B9D-A9C0-2644-B446-5EA3501C2B5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="22">
   <si>
     <t>tests/data/</t>
   </si>
@@ -92,6 +92,12 @@
   </si>
   <si>
     <t>~/Python/org-alk-sausage-machine</t>
+  </si>
+  <si>
+    <t>Lueker</t>
+  </si>
+  <si>
+    <t>CTNa</t>
   </si>
 </sst>
 </file>
@@ -932,10 +938,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L10"/>
+  <dimension ref="A1:M10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I25" sqref="I25"/>
+      <selection activeCell="N21" sqref="N21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -950,7 +956,7 @@
     <col min="13" max="13" width="15.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -987,8 +993,11 @@
       <c r="L1" t="s">
         <v>13</v>
       </c>
+      <c r="M1" t="s">
+        <v>21</v>
+      </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>19</v>
       </c>
@@ -1020,10 +1029,13 @@
         <v>3.5</v>
       </c>
       <c r="L2" t="s">
-        <v>14</v>
+        <v>20</v>
+      </c>
+      <c r="M2">
+        <v>14.99</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>19</v>
       </c>
@@ -1055,10 +1067,13 @@
         <v>3.5</v>
       </c>
       <c r="L3" t="s">
-        <v>14</v>
+        <v>20</v>
+      </c>
+      <c r="M3">
+        <v>14.99</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>19</v>
       </c>
@@ -1090,10 +1105,13 @@
         <v>3.5</v>
       </c>
       <c r="L4" t="s">
-        <v>14</v>
+        <v>20</v>
+      </c>
+      <c r="M4">
+        <v>14.99</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -1127,8 +1145,11 @@
       <c r="L5" t="s">
         <v>14</v>
       </c>
+      <c r="M5">
+        <v>14.99</v>
+      </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>0</v>
       </c>
@@ -1162,8 +1183,11 @@
       <c r="L6" t="s">
         <v>14</v>
       </c>
+      <c r="M6">
+        <v>14.99</v>
+      </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>0</v>
       </c>
@@ -1197,8 +1221,11 @@
       <c r="L7" t="s">
         <v>14</v>
       </c>
+      <c r="M7">
+        <v>14.99</v>
+      </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>0</v>
       </c>
@@ -1232,8 +1259,11 @@
       <c r="L8" t="s">
         <v>14</v>
       </c>
+      <c r="M8">
+        <v>14.99</v>
+      </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
         <v>15</v>
       </c>

</xml_diff>

<commit_message>
Updated master tit file to final format
</commit_message>
<xml_diff>
--- a/Master_Tit_File.xlsx
+++ b/Master_Tit_File.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ct6g18/Python/org-alk-sausage-machine/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dankerr/Desktop/OrgAlk Code CT NOCS/GitRepos/org-alk-sausage-machine-03_04_22/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66FFC717-CDC4-2649-876B-5BA772EBED4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{DA31C14F-F1EE-D549-8ACA-80A59B14C3A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="titration_table" sheetId="1" r:id="rId1"/>
@@ -32,13 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="20">
-  <si>
-    <t>tests/data/</t>
-  </si>
-  <si>
-    <t>seawater-CRM-144.dat</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t>g_0</t>
   </si>
@@ -73,15 +67,6 @@
     <t>intercept_NaOH</t>
   </si>
   <si>
-    <t>carbonate_K</t>
-  </si>
-  <si>
-    <t>Lueker, Waters etc</t>
-  </si>
-  <si>
-    <t>This is the file name (should be a .xlsx)</t>
-  </si>
-  <si>
     <t>01.09.21.50UM.001.BT_PROCESSED.xlsx</t>
   </si>
   <si>
@@ -92,6 +77,54 @@
   </si>
   <si>
     <t>~/Python/org-alk-sausage-machine</t>
+  </si>
+  <si>
+    <t>CTNa</t>
+  </si>
+  <si>
+    <t>because carbonate_K is false, =0</t>
+  </si>
+  <si>
+    <t>KB</t>
+  </si>
+  <si>
+    <t>K1K2</t>
+  </si>
+  <si>
+    <t>if K1K2 = TRUE and used has specified which constants to used then CTNa will be a user entered value. If K1K2 = FALSE, then CTNa is not used and should automatically be false</t>
+  </si>
+  <si>
+    <t>dissociation constant for boric acid. Set to FALSE in our case as we are using synthetic seawater</t>
+  </si>
+  <si>
+    <t>I_HCl</t>
+  </si>
+  <si>
+    <t>I_NaOH</t>
+  </si>
+  <si>
+    <t>KX_1</t>
+  </si>
+  <si>
+    <t>KX_2</t>
+  </si>
+  <si>
+    <t>KX_3</t>
+  </si>
+  <si>
+    <t>PT</t>
+  </si>
+  <si>
+    <t>SiT</t>
+  </si>
+  <si>
+    <t>user supplied value of total phosphate. Can be any value &gt;0 or FALSE if not used</t>
+  </si>
+  <si>
+    <t>user supplied value of total silicate. Can be any value &gt;0 or FALSE if not used</t>
+  </si>
+  <si>
+    <t>carbonate system dissociation constants K1 and K2. Leaving as FALSE in this case. User should specify what set of constants to use eg Lueker, Cai, Millero etc</t>
   </si>
 </sst>
 </file>
@@ -575,8 +608,14 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -932,313 +971,322 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L10"/>
+  <dimension ref="A1:W18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I25" sqref="I25"/>
+      <selection activeCell="F2" sqref="F2:G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="31.1640625" customWidth="1"/>
-    <col min="2" max="2" width="48.6640625" customWidth="1"/>
-    <col min="8" max="8" width="15.6640625" customWidth="1"/>
-    <col min="9" max="9" width="14.33203125" customWidth="1"/>
-    <col min="10" max="10" width="14.5" customWidth="1"/>
-    <col min="11" max="11" width="15.1640625" customWidth="1"/>
-    <col min="12" max="12" width="14.83203125" customWidth="1"/>
-    <col min="13" max="13" width="15.83203125" customWidth="1"/>
+    <col min="1" max="1" width="31.1640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="48.6640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="20.5" style="1" customWidth="1"/>
+    <col min="4" max="5" width="8.83203125" style="1"/>
+    <col min="6" max="6" width="15.33203125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="14" style="1" customWidth="1"/>
+    <col min="8" max="8" width="15.5" style="1" customWidth="1"/>
+    <col min="9" max="9" width="13.1640625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="15.6640625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="14.33203125" style="1" customWidth="1"/>
+    <col min="12" max="12" width="14.5" style="1" customWidth="1"/>
+    <col min="13" max="16" width="15.1640625" style="1" customWidth="1"/>
+    <col min="17" max="20" width="14.83203125" style="1" customWidth="1"/>
+    <col min="21" max="21" width="15.83203125" style="1" customWidth="1"/>
+    <col min="22" max="22" width="15.5" style="1" customWidth="1"/>
+    <col min="23" max="23" width="16.33203125" style="1" customWidth="1"/>
+    <col min="24" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B1" t="s">
+      <c r="G1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" t="s">
+      <c r="I1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G1" t="s">
-        <v>7</v>
-      </c>
-      <c r="H1" t="s">
+      <c r="L1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="I1" t="s">
+      <c r="M1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="J1" t="s">
+      <c r="N1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="1">
+        <v>35</v>
+      </c>
+      <c r="D2" s="1">
+        <v>79.594700000000003</v>
+      </c>
+      <c r="E2" s="1">
+        <v>27.501799999999999</v>
+      </c>
+      <c r="F2" s="1">
+        <v>0.10060392</v>
+      </c>
+      <c r="G2" s="1">
+        <v>0.10060392</v>
+      </c>
+      <c r="H2" s="1">
+        <v>8.2744091000000006E-2</v>
+      </c>
+      <c r="I2" s="1">
+        <v>8.2744091000000006E-2</v>
+      </c>
+      <c r="J2" s="1">
+        <v>1.0211919300000001</v>
+      </c>
+      <c r="K2" s="1">
+        <v>-8.9579999999999998E-4</v>
+      </c>
+      <c r="L2" s="1">
+        <v>1.2706834499999999</v>
+      </c>
+      <c r="M2" s="1">
+        <v>-1.4702658E-2</v>
+      </c>
+      <c r="N2" s="1">
+        <f>10^-4.5</f>
+        <v>3.1622776601683748E-5</v>
+      </c>
+      <c r="O2" s="1">
+        <f>10^-5.25</f>
+        <v>5.6234132519034836E-6</v>
+      </c>
+      <c r="P2" s="1">
+        <f>10^-5.5</f>
+        <v>3.1622776601683767E-6</v>
+      </c>
+      <c r="Q2" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="S2" s="1">
+        <v>0</v>
+      </c>
+      <c r="T2" s="1">
+        <v>0</v>
+      </c>
+      <c r="W2" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="B3" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="B4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="K1" t="s">
-        <v>12</v>
-      </c>
-      <c r="L1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+    </row>
+    <row r="5" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="Q5" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="R5" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C2">
-        <v>33.570999999999998</v>
-      </c>
-      <c r="E2">
-        <v>100</v>
-      </c>
-      <c r="F2">
-        <v>10</v>
-      </c>
-      <c r="G2">
-        <v>2031.53</v>
-      </c>
-      <c r="H2">
-        <v>0.31</v>
-      </c>
-      <c r="I2">
-        <v>2.5</v>
-      </c>
-      <c r="J2">
-        <v>0.21</v>
-      </c>
-      <c r="K2">
-        <v>3.5</v>
-      </c>
-      <c r="L2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C3">
-        <v>33.573</v>
-      </c>
-      <c r="E3">
-        <v>1000</v>
-      </c>
-      <c r="F3">
-        <v>10</v>
-      </c>
-      <c r="G3">
-        <v>2031.53</v>
-      </c>
-      <c r="H3">
-        <v>0.31</v>
-      </c>
-      <c r="I3">
-        <v>2.5</v>
-      </c>
-      <c r="J3">
-        <v>0.21</v>
-      </c>
-      <c r="K3">
-        <v>3.5</v>
-      </c>
-      <c r="L3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C4">
-        <v>33.570999999999998</v>
-      </c>
-      <c r="E4">
-        <v>100</v>
-      </c>
-      <c r="F4">
-        <v>10</v>
-      </c>
-      <c r="G4">
-        <v>2031.53</v>
-      </c>
-      <c r="H4">
-        <v>0.31</v>
-      </c>
-      <c r="I4">
-        <v>2.5</v>
-      </c>
-      <c r="J4">
-        <v>0.21</v>
-      </c>
-      <c r="K4">
-        <v>3.5</v>
-      </c>
-      <c r="L4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C5">
-        <v>33.570999999999998</v>
-      </c>
-      <c r="E5">
-        <v>100</v>
-      </c>
-      <c r="F5">
-        <v>10</v>
-      </c>
-      <c r="G5">
-        <v>2031.53</v>
-      </c>
-      <c r="H5">
-        <v>0.31</v>
-      </c>
-      <c r="I5">
-        <v>2.5</v>
-      </c>
-      <c r="J5">
-        <v>0.21</v>
-      </c>
-      <c r="K5">
-        <v>3.5</v>
-      </c>
-      <c r="L5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>0</v>
-      </c>
-      <c r="B6" t="s">
-        <v>1</v>
-      </c>
-      <c r="C6">
-        <v>33.570999999999998</v>
-      </c>
-      <c r="E6">
-        <v>100</v>
-      </c>
-      <c r="F6">
-        <v>10</v>
-      </c>
-      <c r="G6">
-        <v>2031.53</v>
-      </c>
-      <c r="H6">
-        <v>0.31</v>
-      </c>
-      <c r="I6">
-        <v>2.5</v>
-      </c>
-      <c r="J6">
-        <v>0.21</v>
-      </c>
-      <c r="K6">
-        <v>3.5</v>
-      </c>
-      <c r="L6" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>0</v>
-      </c>
-      <c r="B7" t="s">
-        <v>1</v>
-      </c>
-      <c r="C7">
-        <v>33.570999999999998</v>
-      </c>
-      <c r="E7">
-        <v>100</v>
-      </c>
-      <c r="F7">
-        <v>10</v>
-      </c>
-      <c r="G7">
-        <v>2031.53</v>
-      </c>
-      <c r="H7">
-        <v>0.31</v>
-      </c>
-      <c r="I7">
-        <v>2.5</v>
-      </c>
-      <c r="J7">
-        <v>0.21</v>
-      </c>
-      <c r="K7">
-        <v>3.5</v>
-      </c>
-      <c r="L7" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>0</v>
-      </c>
-      <c r="B8" t="s">
-        <v>1</v>
-      </c>
-      <c r="C8">
-        <v>33.570999999999998</v>
-      </c>
-      <c r="E8">
-        <v>100</v>
-      </c>
-      <c r="F8">
-        <v>10</v>
-      </c>
-      <c r="G8">
-        <v>2031.53</v>
-      </c>
-      <c r="H8">
-        <v>0.31</v>
-      </c>
-      <c r="I8">
-        <v>2.5</v>
-      </c>
-      <c r="J8">
-        <v>0.21</v>
-      </c>
-      <c r="K8">
-        <v>3.5</v>
-      </c>
-      <c r="L8" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B10" t="s">
-        <v>15</v>
-      </c>
+      <c r="S5" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="T5" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="U5" s="2"/>
+      <c r="V5" s="2"/>
+      <c r="W5" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="Q6" s="2"/>
+      <c r="R6" s="2"/>
+      <c r="S6" s="2"/>
+      <c r="T6" s="2"/>
+      <c r="U6" s="2"/>
+      <c r="V6" s="2"/>
+      <c r="W6" s="2"/>
+    </row>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="Q7" s="2"/>
+      <c r="R7" s="2"/>
+      <c r="S7" s="2"/>
+      <c r="T7" s="2"/>
+      <c r="U7" s="2"/>
+      <c r="V7" s="2"/>
+      <c r="W7" s="2"/>
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="Q8" s="2"/>
+      <c r="R8" s="2"/>
+      <c r="S8" s="2"/>
+      <c r="T8" s="2"/>
+      <c r="U8" s="2"/>
+      <c r="V8" s="2"/>
+      <c r="W8" s="2"/>
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="Q9" s="2"/>
+      <c r="R9" s="2"/>
+      <c r="S9" s="2"/>
+      <c r="T9" s="2"/>
+      <c r="U9" s="2"/>
+      <c r="V9" s="2"/>
+      <c r="W9" s="2"/>
+    </row>
+    <row r="10" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="Q10" s="2"/>
+      <c r="R10" s="2"/>
+      <c r="S10" s="2"/>
+      <c r="T10" s="2"/>
+      <c r="U10" s="2"/>
+      <c r="V10" s="2"/>
+      <c r="W10" s="2"/>
+    </row>
+    <row r="11" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="Q11" s="2"/>
+      <c r="R11" s="2"/>
+      <c r="S11" s="2"/>
+      <c r="T11" s="2"/>
+      <c r="U11" s="2"/>
+      <c r="V11" s="2"/>
+      <c r="W11" s="2"/>
+    </row>
+    <row r="12" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="Q12" s="2"/>
+      <c r="R12" s="2"/>
+      <c r="S12" s="2"/>
+      <c r="T12" s="2"/>
+      <c r="U12" s="2"/>
+      <c r="V12" s="2"/>
+      <c r="W12" s="2"/>
+    </row>
+    <row r="13" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="Q13" s="2"/>
+      <c r="R13" s="2"/>
+      <c r="S13" s="2"/>
+      <c r="T13" s="2"/>
+      <c r="U13" s="2"/>
+      <c r="V13" s="2"/>
+      <c r="W13" s="2"/>
+    </row>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="Q14" s="2"/>
+      <c r="R14" s="2"/>
+      <c r="S14" s="2"/>
+      <c r="T14" s="2"/>
+      <c r="U14" s="2"/>
+      <c r="V14" s="2"/>
+      <c r="W14" s="2"/>
+    </row>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="Q15" s="2"/>
+      <c r="R15" s="2"/>
+      <c r="S15" s="2"/>
+      <c r="T15" s="2"/>
+      <c r="U15" s="2"/>
+      <c r="V15" s="2"/>
+      <c r="W15" s="2"/>
+    </row>
+    <row r="16" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="Q16" s="2"/>
+      <c r="R16" s="2"/>
+      <c r="S16" s="2"/>
+      <c r="T16" s="2"/>
+      <c r="U16" s="2"/>
+      <c r="V16" s="2"/>
+      <c r="W16" s="2"/>
+    </row>
+    <row r="17" spans="17:23" x14ac:dyDescent="0.2">
+      <c r="Q17" s="2"/>
+      <c r="R17" s="2"/>
+      <c r="S17" s="2"/>
+      <c r="T17" s="2"/>
+      <c r="U17" s="2"/>
+      <c r="V17" s="2"/>
+      <c r="W17" s="2"/>
+    </row>
+    <row r="18" spans="17:23" x14ac:dyDescent="0.2">
+      <c r="Q18" s="2"/>
+      <c r="R18" s="2"/>
+      <c r="S18" s="2"/>
+      <c r="T18" s="2"/>
+      <c r="U18" s="2"/>
+      <c r="V18" s="2"/>
+      <c r="W18" s="2"/>
     </row>
   </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="W5:W18"/>
+    <mergeCell ref="Q5:Q18"/>
+    <mergeCell ref="R5:R18"/>
+    <mergeCell ref="U5:U18"/>
+    <mergeCell ref="V5:V18"/>
+    <mergeCell ref="S5:S18"/>
+    <mergeCell ref="T5:T18"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fixed problems with merge
</commit_message>
<xml_diff>
--- a/Master_Tit_File.xlsx
+++ b/Master_Tit_File.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ct6g18/Python/org-alk-sausage-machine/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92EA2B9D-A9C0-2644-B446-5EA3501C2B5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{389EF617-CE51-4B40-A325-D288CABB3B2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="200" yWindow="960" windowWidth="16980" windowHeight="19900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="titration_table" sheetId="1" r:id="rId1"/>
@@ -32,13 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="22">
-  <si>
-    <t>tests/data/</t>
-  </si>
-  <si>
-    <t>seawater-CRM-144.dat</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>g_0</t>
   </si>
@@ -73,15 +67,6 @@
     <t>intercept_NaOH</t>
   </si>
   <si>
-    <t>carbonate_K</t>
-  </si>
-  <si>
-    <t>Lueker, Waters etc</t>
-  </si>
-  <si>
-    <t>This is the file name (should be a .xlsx)</t>
-  </si>
-  <si>
     <t>01.09.21.50UM.001.BT_PROCESSED.xlsx</t>
   </si>
   <si>
@@ -94,10 +79,49 @@
     <t>~/Python/org-alk-sausage-machine</t>
   </si>
   <si>
-    <t>Lueker</t>
-  </si>
-  <si>
     <t>CTNa</t>
+  </si>
+  <si>
+    <t>KB</t>
+  </si>
+  <si>
+    <t>K1K2</t>
+  </si>
+  <si>
+    <t>if K1K2 = TRUE and used has specified which constants to used then CTNa will be a user entered value. If K1K2 = FALSE, then CTNa is not used and should automatically be false</t>
+  </si>
+  <si>
+    <t>dissociation constant for boric acid. Set to FALSE in our case as we are using synthetic seawater</t>
+  </si>
+  <si>
+    <t>I_HCl</t>
+  </si>
+  <si>
+    <t>I_NaOH</t>
+  </si>
+  <si>
+    <t>KX_1</t>
+  </si>
+  <si>
+    <t>KX_2</t>
+  </si>
+  <si>
+    <t>KX_3</t>
+  </si>
+  <si>
+    <t>PT</t>
+  </si>
+  <si>
+    <t>SiT</t>
+  </si>
+  <si>
+    <t>user supplied value of total phosphate. Can be any value &gt;0 or FALSE if not used</t>
+  </si>
+  <si>
+    <t>user supplied value of total silicate. Can be any value &gt;0 or FALSE if not used</t>
+  </si>
+  <si>
+    <t>carbonate system dissociation constants K1 and K2. Leaving as FALSE in this case. User should specify what set of constants to use eg Lueker, Cai, Millero etc</t>
   </si>
 </sst>
 </file>
@@ -581,8 +605,14 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -938,337 +968,322 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M10"/>
+  <dimension ref="A1:W18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N21" sqref="N21"/>
+    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
+      <selection activeCell="R2" sqref="R2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="31.1640625" customWidth="1"/>
-    <col min="2" max="2" width="48.6640625" customWidth="1"/>
-    <col min="8" max="8" width="15.6640625" customWidth="1"/>
-    <col min="9" max="9" width="14.33203125" customWidth="1"/>
-    <col min="10" max="10" width="14.5" customWidth="1"/>
-    <col min="11" max="11" width="15.1640625" customWidth="1"/>
-    <col min="12" max="12" width="14.83203125" customWidth="1"/>
-    <col min="13" max="13" width="15.83203125" customWidth="1"/>
+    <col min="1" max="1" width="31.1640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="48.6640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="20.5" style="1" customWidth="1"/>
+    <col min="4" max="5" width="8.83203125" style="1"/>
+    <col min="6" max="6" width="15.33203125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="14" style="1" customWidth="1"/>
+    <col min="8" max="8" width="15.5" style="1" customWidth="1"/>
+    <col min="9" max="9" width="13.1640625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="15.6640625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="14.33203125" style="1" customWidth="1"/>
+    <col min="12" max="12" width="14.5" style="1" customWidth="1"/>
+    <col min="13" max="16" width="15.1640625" style="1" customWidth="1"/>
+    <col min="17" max="20" width="14.83203125" style="1" customWidth="1"/>
+    <col min="21" max="21" width="15.83203125" style="1" customWidth="1"/>
+    <col min="22" max="22" width="15.5" style="1" customWidth="1"/>
+    <col min="23" max="23" width="16.33203125" style="1" customWidth="1"/>
+    <col min="24" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B1" t="s">
+      <c r="G1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" t="s">
+      <c r="I1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G1" t="s">
-        <v>7</v>
-      </c>
-      <c r="H1" t="s">
+      <c r="L1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="I1" t="s">
+      <c r="M1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="J1" t="s">
+      <c r="N1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="1">
+        <v>35</v>
+      </c>
+      <c r="D2" s="1">
+        <v>79.594700000000003</v>
+      </c>
+      <c r="E2" s="1">
+        <v>27.501799999999999</v>
+      </c>
+      <c r="F2" s="1">
+        <v>0.10060392</v>
+      </c>
+      <c r="G2" s="1">
+        <v>0.10060392</v>
+      </c>
+      <c r="H2" s="1">
+        <v>8.2744091000000006E-2</v>
+      </c>
+      <c r="I2" s="1">
+        <v>8.2744091000000006E-2</v>
+      </c>
+      <c r="J2" s="1">
+        <v>-8.9579999999999998E-4</v>
+      </c>
+      <c r="K2" s="1">
+        <v>1.0211919300000001</v>
+      </c>
+      <c r="L2" s="1">
+        <v>-1.4702658E-2</v>
+      </c>
+      <c r="M2" s="1">
+        <v>1.2706834499999999</v>
+      </c>
+      <c r="N2" s="1">
+        <f>10^-4.5</f>
+        <v>3.1622776601683748E-5</v>
+      </c>
+      <c r="O2" s="1">
+        <f>10^-5.25</f>
+        <v>5.6234132519034836E-6</v>
+      </c>
+      <c r="P2" s="1">
+        <f>10^-5.5</f>
+        <v>3.1622776601683767E-6</v>
+      </c>
+      <c r="Q2" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="R2" s="1">
+        <v>0</v>
+      </c>
+      <c r="S2" s="1">
+        <v>0</v>
+      </c>
+      <c r="T2" s="1">
+        <v>0</v>
+      </c>
+      <c r="W2" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="B3" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="B4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="K1" t="s">
-        <v>12</v>
-      </c>
-      <c r="L1" t="s">
-        <v>13</v>
-      </c>
-      <c r="M1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+    </row>
+    <row r="5" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="Q5" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="R5" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="S5" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="T5" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="U5" s="2"/>
+      <c r="V5" s="2"/>
+      <c r="W5" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C2">
-        <v>33.570999999999998</v>
-      </c>
-      <c r="E2">
-        <v>100</v>
-      </c>
-      <c r="F2">
-        <v>10</v>
-      </c>
-      <c r="G2">
-        <v>2031.53</v>
-      </c>
-      <c r="H2">
-        <v>0.31</v>
-      </c>
-      <c r="I2">
-        <v>2.5</v>
-      </c>
-      <c r="J2">
-        <v>0.21</v>
-      </c>
-      <c r="K2">
-        <v>3.5</v>
-      </c>
-      <c r="L2" t="s">
-        <v>20</v>
-      </c>
-      <c r="M2">
-        <v>14.99</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C3">
-        <v>33.573</v>
-      </c>
-      <c r="E3">
-        <v>1000</v>
-      </c>
-      <c r="F3">
-        <v>10</v>
-      </c>
-      <c r="G3">
-        <v>2031.53</v>
-      </c>
-      <c r="H3">
-        <v>0.31</v>
-      </c>
-      <c r="I3">
-        <v>2.5</v>
-      </c>
-      <c r="J3">
-        <v>0.21</v>
-      </c>
-      <c r="K3">
-        <v>3.5</v>
-      </c>
-      <c r="L3" t="s">
-        <v>20</v>
-      </c>
-      <c r="M3">
-        <v>14.99</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C4">
-        <v>33.570999999999998</v>
-      </c>
-      <c r="E4">
-        <v>100</v>
-      </c>
-      <c r="F4">
-        <v>10</v>
-      </c>
-      <c r="G4">
-        <v>2031.53</v>
-      </c>
-      <c r="H4">
-        <v>0.31</v>
-      </c>
-      <c r="I4">
-        <v>2.5</v>
-      </c>
-      <c r="J4">
-        <v>0.21</v>
-      </c>
-      <c r="K4">
-        <v>3.5</v>
-      </c>
-      <c r="L4" t="s">
-        <v>20</v>
-      </c>
-      <c r="M4">
-        <v>14.99</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C5">
-        <v>33.570999999999998</v>
-      </c>
-      <c r="E5">
-        <v>100</v>
-      </c>
-      <c r="F5">
-        <v>10</v>
-      </c>
-      <c r="G5">
-        <v>2031.53</v>
-      </c>
-      <c r="H5">
-        <v>0.31</v>
-      </c>
-      <c r="I5">
-        <v>2.5</v>
-      </c>
-      <c r="J5">
-        <v>0.21</v>
-      </c>
-      <c r="K5">
-        <v>3.5</v>
-      </c>
-      <c r="L5" t="s">
-        <v>14</v>
-      </c>
-      <c r="M5">
-        <v>14.99</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>0</v>
-      </c>
-      <c r="B6" t="s">
-        <v>1</v>
-      </c>
-      <c r="C6">
-        <v>33.570999999999998</v>
-      </c>
-      <c r="E6">
-        <v>100</v>
-      </c>
-      <c r="F6">
-        <v>10</v>
-      </c>
-      <c r="G6">
-        <v>2031.53</v>
-      </c>
-      <c r="H6">
-        <v>0.31</v>
-      </c>
-      <c r="I6">
-        <v>2.5</v>
-      </c>
-      <c r="J6">
-        <v>0.21</v>
-      </c>
-      <c r="K6">
-        <v>3.5</v>
-      </c>
-      <c r="L6" t="s">
-        <v>14</v>
-      </c>
-      <c r="M6">
-        <v>14.99</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>0</v>
-      </c>
-      <c r="B7" t="s">
-        <v>1</v>
-      </c>
-      <c r="C7">
-        <v>33.570999999999998</v>
-      </c>
-      <c r="E7">
-        <v>100</v>
-      </c>
-      <c r="F7">
-        <v>10</v>
-      </c>
-      <c r="G7">
-        <v>2031.53</v>
-      </c>
-      <c r="H7">
-        <v>0.31</v>
-      </c>
-      <c r="I7">
-        <v>2.5</v>
-      </c>
-      <c r="J7">
-        <v>0.21</v>
-      </c>
-      <c r="K7">
-        <v>3.5</v>
-      </c>
-      <c r="L7" t="s">
-        <v>14</v>
-      </c>
-      <c r="M7">
-        <v>14.99</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>0</v>
-      </c>
-      <c r="B8" t="s">
-        <v>1</v>
-      </c>
-      <c r="C8">
-        <v>33.570999999999998</v>
-      </c>
-      <c r="E8">
-        <v>100</v>
-      </c>
-      <c r="F8">
-        <v>10</v>
-      </c>
-      <c r="G8">
-        <v>2031.53</v>
-      </c>
-      <c r="H8">
-        <v>0.31</v>
-      </c>
-      <c r="I8">
-        <v>2.5</v>
-      </c>
-      <c r="J8">
-        <v>0.21</v>
-      </c>
-      <c r="K8">
-        <v>3.5</v>
-      </c>
-      <c r="L8" t="s">
-        <v>14</v>
-      </c>
-      <c r="M8">
-        <v>14.99</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B10" t="s">
-        <v>15</v>
-      </c>
+    </row>
+    <row r="6" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="Q6" s="2"/>
+      <c r="R6" s="2"/>
+      <c r="S6" s="2"/>
+      <c r="T6" s="2"/>
+      <c r="U6" s="2"/>
+      <c r="V6" s="2"/>
+      <c r="W6" s="2"/>
+    </row>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="Q7" s="2"/>
+      <c r="R7" s="2"/>
+      <c r="S7" s="2"/>
+      <c r="T7" s="2"/>
+      <c r="U7" s="2"/>
+      <c r="V7" s="2"/>
+      <c r="W7" s="2"/>
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="Q8" s="2"/>
+      <c r="R8" s="2"/>
+      <c r="S8" s="2"/>
+      <c r="T8" s="2"/>
+      <c r="U8" s="2"/>
+      <c r="V8" s="2"/>
+      <c r="W8" s="2"/>
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="Q9" s="2"/>
+      <c r="R9" s="2"/>
+      <c r="S9" s="2"/>
+      <c r="T9" s="2"/>
+      <c r="U9" s="2"/>
+      <c r="V9" s="2"/>
+      <c r="W9" s="2"/>
+    </row>
+    <row r="10" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="Q10" s="2"/>
+      <c r="R10" s="2"/>
+      <c r="S10" s="2"/>
+      <c r="T10" s="2"/>
+      <c r="U10" s="2"/>
+      <c r="V10" s="2"/>
+      <c r="W10" s="2"/>
+    </row>
+    <row r="11" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="Q11" s="2"/>
+      <c r="R11" s="2"/>
+      <c r="S11" s="2"/>
+      <c r="T11" s="2"/>
+      <c r="U11" s="2"/>
+      <c r="V11" s="2"/>
+      <c r="W11" s="2"/>
+    </row>
+    <row r="12" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="Q12" s="2"/>
+      <c r="R12" s="2"/>
+      <c r="S12" s="2"/>
+      <c r="T12" s="2"/>
+      <c r="U12" s="2"/>
+      <c r="V12" s="2"/>
+      <c r="W12" s="2"/>
+    </row>
+    <row r="13" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="Q13" s="2"/>
+      <c r="R13" s="2"/>
+      <c r="S13" s="2"/>
+      <c r="T13" s="2"/>
+      <c r="U13" s="2"/>
+      <c r="V13" s="2"/>
+      <c r="W13" s="2"/>
+    </row>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="Q14" s="2"/>
+      <c r="R14" s="2"/>
+      <c r="S14" s="2"/>
+      <c r="T14" s="2"/>
+      <c r="U14" s="2"/>
+      <c r="V14" s="2"/>
+      <c r="W14" s="2"/>
+    </row>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="Q15" s="2"/>
+      <c r="R15" s="2"/>
+      <c r="S15" s="2"/>
+      <c r="T15" s="2"/>
+      <c r="U15" s="2"/>
+      <c r="V15" s="2"/>
+      <c r="W15" s="2"/>
+    </row>
+    <row r="16" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="Q16" s="2"/>
+      <c r="R16" s="2"/>
+      <c r="S16" s="2"/>
+      <c r="T16" s="2"/>
+      <c r="U16" s="2"/>
+      <c r="V16" s="2"/>
+      <c r="W16" s="2"/>
+    </row>
+    <row r="17" spans="17:23" x14ac:dyDescent="0.2">
+      <c r="Q17" s="2"/>
+      <c r="R17" s="2"/>
+      <c r="S17" s="2"/>
+      <c r="T17" s="2"/>
+      <c r="U17" s="2"/>
+      <c r="V17" s="2"/>
+      <c r="W17" s="2"/>
+    </row>
+    <row r="18" spans="17:23" x14ac:dyDescent="0.2">
+      <c r="Q18" s="2"/>
+      <c r="R18" s="2"/>
+      <c r="S18" s="2"/>
+      <c r="T18" s="2"/>
+      <c r="U18" s="2"/>
+      <c r="V18" s="2"/>
+      <c r="W18" s="2"/>
     </row>
   </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="W5:W18"/>
+    <mergeCell ref="Q5:Q18"/>
+    <mergeCell ref="R5:R18"/>
+    <mergeCell ref="U5:U18"/>
+    <mergeCell ref="V5:V18"/>
+    <mergeCell ref="S5:S18"/>
+    <mergeCell ref="T5:T18"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>